<commit_message>
psychopy file lab 5 updates
</commit_message>
<xml_diff>
--- a/05-adaptive-methods/adaptive-methods/staircase_parameters.xlsx
+++ b/05-adaptive-methods/adaptive-methods/staircase_parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://indiana-my.sharepoint.com/personal/kbonnen_iu_edu/Documents/Courses/V768-Measuring-Perception/V768-Psychophysics-labs/05-adaptive-methods/adaptive-methods/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="50" documentId="8_{44A74B6C-5AB4-1D45-9146-C88ED770F71E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{929045D6-2403-2E40-B491-B48D76B3C569}"/>
+  <xr:revisionPtr revIDLastSave="52" documentId="8_{44A74B6C-5AB4-1D45-9146-C88ED770F71E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B873DBEF-B543-7B4A-9E3D-78BC276C58CF}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="25780" windowHeight="13860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -758,7 +758,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -813,7 +813,7 @@
         <v>15</v>
       </c>
       <c r="E2">
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -839,7 +839,7 @@
         <v>-12</v>
       </c>
       <c r="D3">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="E3">
         <v>-15</v>
@@ -937,12 +937,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B9F5CAB0486A994CA2C3B13E059EF2AE" ma:contentTypeVersion="0" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="8645ec4a60d0c8c7009d2d6675847a91">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="636d7205651659ec4fcda0bcbde9384b">
     <xsd:element name="properties">
@@ -1056,6 +1050,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3744155D-8FAB-4E67-B5E0-C7FDBFB3715D}">
   <ds:schemaRefs>
@@ -1065,21 +1065,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3725960-8A89-4E70-9C40-340E0EDB6403}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EFF1C174-6AC6-4774-A736-3226A12360E4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1093,4 +1078,19 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3725960-8A89-4E70-9C40-340E0EDB6403}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>